<commit_message>
User CRUD complete + Email portal fixes
</commit_message>
<xml_diff>
--- a/Email Upload Template.xlsx
+++ b/Email Upload Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Padraig\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Padraig\Desktop\Computing Project\ComputingProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36CB352-E7EF-48D5-B7B3-4702014F4056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF162588-BA3F-42C0-8640-03142B9AEAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D66E3EE3-C821-4D7B-9F29-F5B61556DA10}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7360" xr2:uid="{D66E3EE3-C821-4D7B-9F29-F5B61556DA10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="10">
   <si>
     <t>sender</t>
   </si>
@@ -448,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF57300-6ADD-4B5B-8CE7-ADAABF44FE8A}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -503,10 +503,310 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{F2DEA0FB-FED0-4704-B956-818CAC34A5BA}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{4692E147-837B-45B6-8B68-99B71174EF7B}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{05DE8213-408E-4B13-A9EA-54C1A045C5D0}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{46E0077D-45DC-4781-9EA8-0C34A79CDA2B}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{885F005C-19F0-462A-9A9A-459B28ADA16E}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{545AED5B-BE54-458D-9563-63467C3C006C}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{1F82104C-E3BB-4059-8CA6-02DE6EC5E501}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{35D7D12F-621F-43A4-A471-82292C5CD397}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{6356468A-497D-410E-AE20-BAF16AB792A0}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{4371E658-48AE-4E02-9B2B-AF8929F93333}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{9FB1544C-081D-4B21-BDDF-E2101BC6F8AB}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{B38247C6-DE1E-4595-9550-A727E72ACF7C}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{0F1348FD-1739-45DB-B192-09623B7FA105}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{1325ACC6-A042-4534-8FBA-AFC4F1DE0211}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{9DA557E1-2ED1-4C7A-8175-7A3909423F67}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{98A3A343-9E7D-4F40-ADB2-756E557B1B47}"/>
+    <hyperlink ref="A18" r:id="rId17" xr:uid="{50C1AE0F-F26D-4D8A-B10F-8939BA996B40}"/>
+    <hyperlink ref="A19" r:id="rId18" xr:uid="{3DA26D21-9D77-404E-942D-84D405780826}"/>
+    <hyperlink ref="A20" r:id="rId19" xr:uid="{837E9807-1570-4EDA-A38A-E32EB9D097BE}"/>
+    <hyperlink ref="A21" r:id="rId20" xr:uid="{D3E1A5D6-96F8-4E25-932E-FFA59E3981E6}"/>
+    <hyperlink ref="A22" r:id="rId21" xr:uid="{33369F2A-65C5-41A9-A0E1-EF74C169BAAE}"/>
+    <hyperlink ref="A23" r:id="rId22" xr:uid="{D730ED8E-13A9-46F7-A851-19E8CBECB142}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>